<commit_message>
Validating the statutory rates
</commit_message>
<xml_diff>
--- a/tax_deficit_simulator/data/statutory_rates.xlsx
+++ b/tax_deficit_simulator/data/statutory_rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Paul-Emmanuel/Desktop/EU Tax Observatory/4. Own Work/0. Tax Deficit/Platform/tax_deficit_simulator/tax_deficit_simulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27FCF02-FB43-C44E-BB1C-E35FF9D217EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E27B0A7-869B-794C-894A-081ECE883403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Temporary statutory tax rates for 2018
</commit_message>
<xml_diff>
--- a/tax_deficit_simulator/data/statutory_rates.xlsx
+++ b/tax_deficit_simulator/data/statutory_rates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Paul-Emmanuel/Desktop/EU Tax Observatory/4. Own Work/0. Tax Deficit/Platform/tax_deficit_simulator/tax_deficit_simulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E27B0A7-869B-794C-894A-081ECE883403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFBCB16-888E-FD4B-8059-CC3EFDED2963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t>ABW</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t>statrate17</t>
+  </si>
+  <si>
+    <t>statrate18</t>
   </si>
 </sst>
 </file>
@@ -949,15 +952,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:D187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D1:D187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>186</v>
       </c>
@@ -967,8 +970,11 @@
       <c r="C1" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -978,8 +984,11 @@
       <c r="C2" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -989,8 +998,11 @@
       <c r="C3" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1000,8 +1012,11 @@
       <c r="C4" s="1">
         <v>0.28210000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="1">
+        <v>0.28210000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1011,8 +1026,11 @@
       <c r="C5" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1020,8 +1038,11 @@
       <c r="C6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1031,8 +1052,11 @@
       <c r="C7" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1042,8 +1066,11 @@
       <c r="C8" s="1">
         <v>0.28289999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="1">
+        <v>0.28289999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1051,8 +1078,11 @@
       <c r="C9" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1062,8 +1092,11 @@
       <c r="C10" s="1">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1073,8 +1106,11 @@
       <c r="C11" s="1">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1084,8 +1120,11 @@
       <c r="C12" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1095,8 +1134,11 @@
       <c r="C13" s="1">
         <v>0.21079999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="1">
+        <v>0.21079999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1104,8 +1146,11 @@
       <c r="C14" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1115,8 +1160,11 @@
       <c r="C15" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1126,8 +1174,11 @@
       <c r="C16" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1135,8 +1186,11 @@
       <c r="C17" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1144,8 +1198,11 @@
       <c r="C18" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1155,8 +1212,11 @@
       <c r="C19" s="1">
         <v>0.33990000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="1">
+        <v>0.33990000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1164,8 +1224,11 @@
       <c r="C20" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1173,8 +1236,11 @@
       <c r="C21" s="1">
         <v>0.27500000000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="1">
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1184,8 +1250,11 @@
       <c r="C22" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1195,8 +1264,11 @@
       <c r="C23" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1206,8 +1278,11 @@
       <c r="C24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1217,8 +1292,11 @@
       <c r="C25" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1228,8 +1306,11 @@
       <c r="C26" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1239,8 +1320,11 @@
       <c r="C27" s="1">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1250,8 +1334,11 @@
       <c r="C28" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1261,8 +1348,11 @@
       <c r="C29" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1272,8 +1362,11 @@
       <c r="C30" s="1">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" s="1">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1283,8 +1376,11 @@
       <c r="C31" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1292,8 +1388,11 @@
       <c r="C32" s="1">
         <v>0.185</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" s="1">
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1303,8 +1402,11 @@
       <c r="C33" s="1">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1314,8 +1416,11 @@
       <c r="C34" s="1">
         <v>0.26500000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" s="1">
+        <v>0.26500000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1325,8 +1430,11 @@
       <c r="C35" s="1">
         <v>0.1777</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" s="1">
+        <v>0.1777</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1336,8 +1444,11 @@
       <c r="C36" s="1">
         <v>0.255</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" s="1">
+        <v>0.255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1347,8 +1458,11 @@
       <c r="C37" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1356,8 +1470,11 @@
       <c r="C38" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1367,8 +1484,11 @@
       <c r="C39" s="1">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1376,15 +1496,19 @@
       <c r="C40" s="1">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1394,8 +1518,11 @@
       <c r="C42" s="1">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" s="1">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1405,8 +1532,11 @@
       <c r="C43" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1416,8 +1546,11 @@
       <c r="C44" s="1">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1427,8 +1560,11 @@
       <c r="C45" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1438,8 +1574,11 @@
       <c r="C46" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1449,8 +1588,11 @@
       <c r="C47" s="1">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1460,8 +1602,11 @@
       <c r="C48" s="1">
         <v>0.2979</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" s="1">
+        <v>0.2979</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1469,8 +1614,11 @@
       <c r="C49" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1478,8 +1626,11 @@
       <c r="C50" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1489,8 +1640,11 @@
       <c r="C51" s="1">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1500,8 +1654,11 @@
       <c r="C52" s="1">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" s="1">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1511,8 +1668,11 @@
       <c r="C53" s="1">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1522,8 +1682,11 @@
       <c r="C54" s="1">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1533,8 +1696,11 @@
       <c r="C55" s="1">
         <v>0.22500000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" s="1">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1544,8 +1710,11 @@
       <c r="C56" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1555,8 +1724,11 @@
       <c r="C57" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1564,8 +1736,11 @@
       <c r="C58" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1575,8 +1750,11 @@
       <c r="C59" s="1">
         <v>0.21410000000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" s="1">
+        <v>0.21410000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1586,8 +1764,11 @@
       <c r="C60" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1597,8 +1778,11 @@
       <c r="C61" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1608,8 +1792,11 @@
       <c r="C62" s="1">
         <v>0.33329999999999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" s="1">
+        <v>0.33329999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1617,8 +1804,11 @@
       <c r="C63" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1628,8 +1818,11 @@
       <c r="C64" s="1">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1639,8 +1832,11 @@
       <c r="C65" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1650,8 +1846,11 @@
       <c r="C66" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1661,8 +1860,11 @@
       <c r="C67" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1672,8 +1874,11 @@
       <c r="C68" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1683,8 +1888,11 @@
       <c r="C69" s="1">
         <v>0.24059999999999998</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69" s="1">
+        <v>0.24059999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1692,8 +1900,11 @@
       <c r="C70" s="1">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70" s="1">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1703,8 +1914,11 @@
       <c r="C71" s="1">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1712,8 +1926,11 @@
       <c r="C72" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -1723,8 +1940,11 @@
       <c r="C73" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -1734,8 +1954,11 @@
       <c r="C74" s="1">
         <v>0.16500000000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74" s="1">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -1745,8 +1968,11 @@
       <c r="C75" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -1756,8 +1982,11 @@
       <c r="C76" s="1">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -1767,8 +1996,11 @@
       <c r="C77" s="1">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -1778,8 +2010,11 @@
       <c r="C78" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -1789,8 +2024,11 @@
       <c r="C79" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -1800,8 +2038,11 @@
       <c r="C80" s="1">
         <v>0.34610000000000002</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80" s="1">
+        <v>0.34610000000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -1811,8 +2052,11 @@
       <c r="C81" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -1822,8 +2066,11 @@
       <c r="C82" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -1833,8 +2080,11 @@
       <c r="C83" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -1844,8 +2094,11 @@
       <c r="C84" s="1">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -1855,8 +2108,11 @@
       <c r="C85" s="1">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -1866,8 +2122,11 @@
       <c r="C86" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -1877,8 +2136,11 @@
       <c r="C87" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -1888,8 +2150,11 @@
       <c r="C88" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -1899,8 +2164,11 @@
       <c r="C89" s="1">
         <v>0.30859999999999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89" s="1">
+        <v>0.30859999999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -1910,8 +2178,11 @@
       <c r="C90" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -1921,8 +2192,11 @@
       <c r="C91" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -1930,8 +2204,11 @@
       <c r="C92" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -1941,8 +2218,11 @@
       <c r="C93" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -1950,8 +2230,11 @@
       <c r="C94" s="1">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -1961,8 +2244,11 @@
       <c r="C95" s="1">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -1972,8 +2258,11 @@
       <c r="C96" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -1983,8 +2272,11 @@
       <c r="C97" s="1">
         <v>0.27979999999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97" s="1">
+        <v>0.27979999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -1994,8 +2286,11 @@
       <c r="C98" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -2005,8 +2300,11 @@
       <c r="C99" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -2014,8 +2312,11 @@
       <c r="C100" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -2025,8 +2326,11 @@
       <c r="C101" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -2036,8 +2340,11 @@
       <c r="C102" s="1">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D102" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -2047,8 +2354,11 @@
       <c r="C103" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D103" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -2058,8 +2368,11 @@
       <c r="C104" s="1">
         <v>0.27079999999999999</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D104" s="1">
+        <v>0.27079999999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -2069,8 +2382,11 @@
       <c r="C105" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D105" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -2080,8 +2396,11 @@
       <c r="C106" s="1">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D106" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -2091,8 +2410,11 @@
       <c r="C107" s="1">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D107" s="1">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -2100,8 +2422,11 @@
       <c r="C108" s="1">
         <v>0.33329999999999999</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D108" s="1">
+        <v>0.33329999999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -2111,8 +2436,11 @@
       <c r="C109" s="1">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D109" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -2120,8 +2448,11 @@
       <c r="C110" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D110" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -2131,8 +2462,11 @@
       <c r="C111" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D111" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -2142,8 +2476,11 @@
       <c r="C112" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D112" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -2153,8 +2490,11 @@
       <c r="C113" s="1">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D113" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -2162,8 +2502,11 @@
       <c r="C114" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D114" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -2173,8 +2516,11 @@
       <c r="C115" s="1">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D115" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -2182,8 +2528,11 @@
       <c r="C116" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D116" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -2193,15 +2542,19 @@
       <c r="C117" s="1">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D117" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>116</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D118" s="1"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -2211,8 +2564,11 @@
       <c r="C119" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D119" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -2222,8 +2578,11 @@
       <c r="C120" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D120" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -2233,8 +2592,11 @@
       <c r="C121" s="1">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D121" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -2244,8 +2606,11 @@
       <c r="C122" s="1">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D122" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -2255,8 +2620,11 @@
       <c r="C123" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D123" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -2264,8 +2632,11 @@
       <c r="C124" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D124" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -2275,8 +2646,11 @@
       <c r="C125" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D125" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -2286,8 +2660,11 @@
       <c r="C126" s="1">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D126" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -2297,8 +2674,11 @@
       <c r="C127" s="1">
         <v>0.33250000000000002</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D127" s="1">
+        <v>0.33250000000000002</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -2308,8 +2688,11 @@
       <c r="C128" s="1">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D128" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -2319,8 +2702,11 @@
       <c r="C129" s="1">
         <v>0.2843</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D129" s="1">
+        <v>0.2843</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -2330,8 +2716,11 @@
       <c r="C130" s="1">
         <v>0.23949999999999999</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D130" s="1">
+        <v>0.23949999999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -2341,8 +2730,11 @@
       <c r="C131" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D131" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>130</v>
       </c>
@@ -2352,8 +2744,11 @@
       <c r="C132" s="1">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D132" s="1">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -2363,8 +2758,11 @@
       <c r="C133" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D133" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -2374,8 +2772,11 @@
       <c r="C134" s="1">
         <v>0.29499999999999998</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D134" s="1">
+        <v>0.29499999999999998</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>133</v>
       </c>
@@ -2385,8 +2786,11 @@
       <c r="C135" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D135" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
@@ -2396,8 +2800,11 @@
       <c r="C136" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D136" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>135</v>
       </c>
@@ -2407,8 +2814,11 @@
       <c r="C137" s="1">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D137" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>136</v>
       </c>
@@ -2418,8 +2828,11 @@
       <c r="C138" s="1">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D138" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>137</v>
       </c>
@@ -2429,8 +2842,11 @@
       <c r="C139" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D139" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>138</v>
       </c>
@@ -2438,8 +2854,11 @@
       <c r="C140" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D140" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>139</v>
       </c>
@@ -2447,8 +2866,11 @@
       <c r="C141" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D141" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>140</v>
       </c>
@@ -2458,8 +2880,11 @@
       <c r="C142" s="1">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D142" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>141</v>
       </c>
@@ -2469,8 +2894,11 @@
       <c r="C143" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D143" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>142</v>
       </c>
@@ -2478,8 +2906,11 @@
       <c r="C144" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D144" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>143</v>
       </c>
@@ -2489,8 +2920,11 @@
       <c r="C145" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D145" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>144</v>
       </c>
@@ -2500,8 +2934,11 @@
       <c r="C146" s="1">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D146" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>145</v>
       </c>
@@ -2509,8 +2946,11 @@
       <c r="C147" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D147" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>146</v>
       </c>
@@ -2520,8 +2960,11 @@
       <c r="C148" s="1">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D148" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>147</v>
       </c>
@@ -2529,8 +2972,11 @@
       <c r="C149" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D149" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>148</v>
       </c>
@@ -2540,8 +2986,11 @@
       <c r="C150" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D150" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>149</v>
       </c>
@@ -2551,8 +3000,11 @@
       <c r="C151" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D151" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>150</v>
       </c>
@@ -2562,8 +3014,11 @@
       <c r="C152" s="1">
         <v>0.27979999999999999</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D152" s="1">
+        <v>0.27979999999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>151</v>
       </c>
@@ -2573,8 +3028,11 @@
       <c r="C153" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D153" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>152</v>
       </c>
@@ -2584,8 +3042,11 @@
       <c r="C154" s="1">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D154" s="1">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>153</v>
       </c>
@@ -2595,8 +3056,11 @@
       <c r="C155" s="1">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D155" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>154</v>
       </c>
@@ -2606,8 +3070,11 @@
       <c r="C156" s="1">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D156" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>155</v>
       </c>
@@ -2617,8 +3084,11 @@
       <c r="C157" s="1">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D157" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>156</v>
       </c>
@@ -2626,8 +3096,11 @@
       <c r="C158" s="1">
         <v>0.27500000000000002</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D158" s="1">
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>157</v>
       </c>
@@ -2637,8 +3110,11 @@
       <c r="C159" s="1">
         <v>0.34499999999999997</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D159" s="1">
+        <v>0.34499999999999997</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>158</v>
       </c>
@@ -2648,8 +3124,11 @@
       <c r="C160" s="1">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D160" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>159</v>
       </c>
@@ -2657,8 +3136,11 @@
       <c r="C161" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D161" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>160</v>
       </c>
@@ -2668,8 +3150,11 @@
       <c r="C162" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D162" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>161</v>
       </c>
@@ -2677,8 +3162,11 @@
       <c r="C163" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D163" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>162</v>
       </c>
@@ -2688,8 +3176,11 @@
       <c r="C164" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D164" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>163</v>
       </c>
@@ -2699,8 +3190,11 @@
       <c r="C165" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D165" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>164</v>
       </c>
@@ -2710,8 +3204,11 @@
       <c r="C166" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D166" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>165</v>
       </c>
@@ -2721,8 +3218,11 @@
       <c r="C167" s="1">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D167" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>166</v>
       </c>
@@ -2732,8 +3232,11 @@
       <c r="C168" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D168" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>167</v>
       </c>
@@ -2743,8 +3246,11 @@
       <c r="C169" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D169" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>168</v>
       </c>
@@ -2754,8 +3260,11 @@
       <c r="C170" s="1">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D170" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>169</v>
       </c>
@@ -2765,8 +3274,11 @@
       <c r="C171" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D171" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>170</v>
       </c>
@@ -2776,8 +3288,11 @@
       <c r="C172" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D172" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>171</v>
       </c>
@@ -2787,8 +3302,11 @@
       <c r="C173" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D173" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>172</v>
       </c>
@@ -2796,8 +3314,11 @@
       <c r="C174" s="1">
         <v>0.32500000000000001</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D174" s="1">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>173</v>
       </c>
@@ -2807,8 +3328,11 @@
       <c r="C175" s="1">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D175" s="1">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>174</v>
       </c>
@@ -2818,8 +3342,11 @@
       <c r="C176" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D176" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>175</v>
       </c>
@@ -2829,8 +3356,11 @@
       <c r="C177" s="1">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D177" s="1">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>176</v>
       </c>
@@ -2840,8 +3370,11 @@
       <c r="C178" s="1">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D178" s="1">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>177</v>
       </c>
@@ -2851,8 +3384,11 @@
       <c r="C179" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D179" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>178</v>
       </c>
@@ -2862,8 +3398,11 @@
       <c r="C180" s="1">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D180" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>179</v>
       </c>
@@ -2873,8 +3412,11 @@
       <c r="C181" s="1">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D181" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>180</v>
       </c>
@@ -2884,8 +3426,11 @@
       <c r="C182" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D182" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>181</v>
       </c>
@@ -2895,8 +3440,11 @@
       <c r="C183" s="1">
         <v>0.28210000000000002</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D183" s="1">
+        <v>0.28210000000000002</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>182</v>
       </c>
@@ -2906,8 +3454,11 @@
       <c r="C184" s="1">
         <v>0.21079999999999999</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D184" s="1">
+        <v>0.21079999999999999</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>183</v>
       </c>
@@ -2917,8 +3468,11 @@
       <c r="C185" s="1">
         <v>0.21410000000000001</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D185" s="1">
+        <v>0.21410000000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>184</v>
       </c>
@@ -2928,8 +3482,11 @@
       <c r="C186" s="1">
         <v>0.28289999999999998</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D186" s="1">
+        <v>0.28289999999999998</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>185</v>
       </c>
@@ -2937,6 +3494,9 @@
         <v>0.23670000000000002</v>
       </c>
       <c r="C187" s="1">
+        <v>0.24059999999999998</v>
+      </c>
+      <c r="D187" s="1">
         <v>0.24059999999999998</v>
       </c>
     </row>

</xml_diff>